<commit_message>
yml update for schedule run
</commit_message>
<xml_diff>
--- a/dataFiles/Signup-Positive.xlsx
+++ b/dataFiles/Signup-Positive.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="5" name="TC_01" state="visible" r:id="rId4"/>
+    <sheet name="TC_01" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -205,34 +205,34 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -244,13 +244,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999938962981048"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -573,15 +573,15 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
@@ -603,7 +603,7 @@
     <col min="18" max="18" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,7 +659,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="60" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -709,7 +709,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" ht="75" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -737,7 +737,7 @@
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" ht="60" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>37</v>
       </c>
@@ -787,7 +787,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>39</v>
       </c>
@@ -815,7 +815,7 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" ht="60" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>43</v>
       </c>
@@ -865,7 +865,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -893,7 +893,7 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" ht="60" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>49</v>
       </c>
@@ -943,7 +943,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>51</v>
       </c>
@@ -971,7 +971,7 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" ht="45" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>55</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>57</v>
       </c>
@@ -1083,6 +1083,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Signup and forgot password fix
</commit_message>
<xml_diff>
--- a/dataFiles/Signup-Positive.xlsx
+++ b/dataFiles/Signup-Positive.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="5" name="TC_01" state="visible" r:id="rId4"/>
+    <sheet name="TC_01" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="85">
   <si>
     <t>Field</t>
   </si>
@@ -215,6 +215,60 @@
   </si>
   <si>
     <t>automationevyw</t>
+  </si>
+  <si>
+    <t>Testdata6</t>
+  </si>
+  <si>
+    <t>Writedata6</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Testdata7</t>
+  </si>
+  <si>
+    <t>Writedata7</t>
+  </si>
+  <si>
+    <t>Friend/Co-Worker</t>
+  </si>
+  <si>
+    <t>Testdata8</t>
+  </si>
+  <si>
+    <t>Writedata8</t>
+  </si>
+  <si>
+    <t>Occupational Health</t>
+  </si>
+  <si>
+    <t>Testdata9</t>
+  </si>
+  <si>
+    <t>Writedata9</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Testdata10</t>
+  </si>
+  <si>
+    <t>Writedata10</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Testdata11</t>
+  </si>
+  <si>
+    <t>Writedata11</t>
+  </si>
+  <si>
+    <t>Benefits Book</t>
   </si>
 </sst>
 </file>
@@ -223,34 +277,34 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -262,13 +316,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999938962981048"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,17 +645,17 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
@@ -612,7 +666,7 @@
     <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="12.85546875" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
@@ -621,7 +675,7 @@
     <col min="19" max="19" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="60" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -733,7 +787,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" ht="75" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
@@ -762,7 +816,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
     </row>
-    <row r="4" ht="60" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>39</v>
       </c>
@@ -815,7 +869,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" ht="45" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>42</v>
       </c>
@@ -844,7 +898,7 @@
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
     </row>
-    <row r="6" ht="60" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
@@ -897,7 +951,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" ht="45" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -926,7 +980,7 @@
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" ht="60" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -979,7 +1033,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" ht="45" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>56</v>
       </c>
@@ -1008,7 +1062,7 @@
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
     </row>
-    <row r="10" ht="45" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>60</v>
       </c>
@@ -1061,7 +1115,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" ht="45" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>63</v>
       </c>
@@ -1090,9 +1144,501 @@
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
     </row>
+    <row r="12" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+    </row>
+    <row r="20" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S20" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S22" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+    </row>
   </sheetData>
   <dataValidations count="15">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 B12 B14 B16 B18 B20 B22">
       <formula1>"Employee,Student"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
@@ -1107,7 +1653,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
       <formula1>"Employee,Student"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M10 M12 M14 M16 M18 M20 M22">
       <formula1>"Benefits Book,Human Resources,Union Representative,Flyer/Handout,Friend/Co-Worker,Radio Ad,Online,Lunch and Learn,Occupational Health,Insurance,other"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2">
@@ -1122,7 +1668,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M8">
       <formula1>"Benefits Book,Human Resources,Union Representative,Flyer/Handout,Friend/Co-Worker,Radio Ad,Online,Lunch and Learn,Occupational Health,Insurance,other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S10 S12 S14 S16 S18 S20 S22">
       <formula1>"Mental Health,Cancer,Chronic Disease,Elder Care"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
@@ -1139,6 +1685,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>